<commit_message>
updated matlab-cpu-gpu spreadsheet - not latest
</commit_message>
<xml_diff>
--- a/src/segment/results/matlab-gpu-cpu/matlab-gpu-cpu.xlsx
+++ b/src/segment/results/matlab-gpu-cpu/matlab-gpu-cpu.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1200" windowWidth="17235" windowHeight="6945"/>
+    <workbookView xWindow="-15" yWindow="4290" windowWidth="19215" windowHeight="4335"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet8 (2)" sheetId="10" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="67">
   <si>
     <t>seg-gpu-timing</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>GPU new</t>
+  </si>
+  <si>
+    <t>from?</t>
   </si>
 </sst>
 </file>
@@ -801,8 +804,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.4185685491972652E-2"/>
-          <c:y val="2.5258854407904891E-2"/>
+          <c:x val="6.459933040199145E-2"/>
+          <c:y val="2.9964736760846065E-2"/>
           <c:w val="0.88792587469676687"/>
           <c:h val="0.87574383202099737"/>
         </c:manualLayout>
@@ -3116,12 +3119,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="58556800"/>
-        <c:axId val="58558336"/>
-        <c:axId val="107083520"/>
+        <c:axId val="53827840"/>
+        <c:axId val="53833728"/>
+        <c:axId val="53822784"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="58556800"/>
+        <c:axId val="53827840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3130,7 +3133,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58558336"/>
+        <c:crossAx val="53833728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3138,7 +3141,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58558336"/>
+        <c:axId val="53833728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3149,12 +3152,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58556800"/>
+        <c:crossAx val="53827840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="107083520"/>
+        <c:axId val="53822784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3163,7 +3166,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58558336"/>
+        <c:crossAx val="53833728"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -3517,8 +3520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6:V6"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5043,10 +5046,14 @@
   <dimension ref="A1:AD6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="55.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -5237,7 +5244,7 @@
         <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>43</v>
@@ -5249,76 +5256,76 @@
         <v>42</v>
       </c>
       <c r="F3">
-        <v>8.3809999999999996E-2</v>
+        <v>1.2329800000000001E-3</v>
       </c>
       <c r="G3">
         <v>135</v>
       </c>
       <c r="H3">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="I3">
-        <v>453</v>
+        <v>348</v>
       </c>
       <c r="J3">
         <v>62</v>
       </c>
       <c r="K3">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="L3">
-        <v>945</v>
+        <v>851</v>
       </c>
       <c r="M3">
-        <v>16775303</v>
+        <v>16775193</v>
       </c>
       <c r="N3">
         <v>40</v>
       </c>
       <c r="O3">
-        <v>525</v>
+        <v>514</v>
       </c>
       <c r="P3">
-        <v>12313</v>
+        <v>2429</v>
       </c>
       <c r="Q3">
-        <v>236</v>
+        <v>160</v>
       </c>
       <c r="R3">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="S3">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T3">
-        <v>4806</v>
+        <v>1370</v>
       </c>
       <c r="U3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="V3">
-        <v>1198</v>
+        <v>1163</v>
       </c>
       <c r="W3">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="X3">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="Y3">
-        <v>26556</v>
+        <v>6776</v>
       </c>
       <c r="Z3">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="AA3">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AB3">
-        <v>5740</v>
+        <v>1536</v>
       </c>
       <c r="AC3">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="AD3" t="s">
         <v>3</v>
@@ -5421,7 +5428,7 @@
         <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
         <v>43</v>
@@ -5433,76 +5440,76 @@
         <v>42</v>
       </c>
       <c r="F5">
-        <v>1.2329800000000001E-3</v>
+        <v>8.3809999999999996E-2</v>
       </c>
       <c r="G5">
         <v>135</v>
       </c>
       <c r="H5">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="I5">
-        <v>348</v>
+        <v>453</v>
       </c>
       <c r="J5">
         <v>62</v>
       </c>
       <c r="K5">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="L5">
-        <v>851</v>
+        <v>945</v>
       </c>
       <c r="M5">
-        <v>16775193</v>
+        <v>16775303</v>
       </c>
       <c r="N5">
         <v>40</v>
       </c>
       <c r="O5">
-        <v>514</v>
+        <v>525</v>
       </c>
       <c r="P5">
-        <v>2429</v>
+        <v>12313</v>
       </c>
       <c r="Q5">
-        <v>160</v>
+        <v>236</v>
       </c>
       <c r="R5">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="S5">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="T5">
-        <v>1370</v>
+        <v>4806</v>
       </c>
       <c r="U5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="V5">
-        <v>1163</v>
+        <v>1198</v>
       </c>
       <c r="W5">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="X5">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="Y5">
-        <v>6776</v>
+        <v>26556</v>
       </c>
       <c r="Z5">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="AA5">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AB5">
-        <v>1536</v>
+        <v>5740</v>
       </c>
       <c r="AC5">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="AD5" t="s">
         <v>3</v>
@@ -5609,7 +5616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="O1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
@@ -6812,7 +6819,7 @@
   <dimension ref="A1:Y13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:X6"/>
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7333,8 +7340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7884,10 +7891,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection sqref="A1:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8088,6 +8095,14 @@
         <v>1425</v>
       </c>
     </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8097,7 +8112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC18"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P5" sqref="P5:AB5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
analyzed results for strong and weak checkpointing IO performance
</commit_message>
<xml_diff>
--- a/src/segment/results/matlab-gpu-cpu/matlab-gpu-cpu.xlsx
+++ b/src/segment/results/matlab-gpu-cpu/matlab-gpu-cpu.xlsx
@@ -828,6 +828,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -981,6 +986,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="92D050"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -1134,6 +1144,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -1287,6 +1302,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -1440,6 +1460,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="92D050"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -1593,6 +1618,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -1746,6 +1776,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -1899,6 +1934,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="92D050"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -2052,6 +2092,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -2205,6 +2250,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -2358,6 +2408,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="92D050"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -2511,6 +2566,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -2664,6 +2724,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -2817,6 +2882,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="92D050"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -2970,6 +3040,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -3119,12 +3194,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="53827840"/>
-        <c:axId val="53833728"/>
-        <c:axId val="53822784"/>
+        <c:axId val="101300096"/>
+        <c:axId val="101301632"/>
+        <c:axId val="101288128"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="53827840"/>
+        <c:axId val="101300096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3133,7 +3208,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53833728"/>
+        <c:crossAx val="101301632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3141,7 +3216,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53833728"/>
+        <c:axId val="101301632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3152,12 +3227,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53827840"/>
+        <c:crossAx val="101300096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="53822784"/>
+        <c:axId val="101288128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3166,7 +3241,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53833728"/>
+        <c:crossAx val="101301632"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -3520,8 +3595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T41" sqref="T41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>